<commit_message>
Corrections of file paths, documentation and outdated entries.
</commit_message>
<xml_diff>
--- a/data/study_search/database_search/processed/post_AS/packages_for_full_text_download/study_set_14.xlsx
+++ b/data/study_search/database_search/processed/post_AS/packages_for_full_text_download/study_set_14.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzprante/GitHub/MORPEP/META_CMP/data/data/study_search/database_search/processed/post_AS/packages_for_full_text_download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBA489F-EA03-6949-A50E-BAE42A747AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BF5A18-4CFD-3B4E-A562-EAF9E07D0F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4980" yWindow="-21100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-300" yWindow="-21100" windowWidth="29040" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -3085,8 +3085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="125" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="AD53" sqref="AD53"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15"/>
@@ -3553,15 +3553,12 @@
         <v>46</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" t="s">
         <v>47</v>
       </c>
       <c r="AG6">
-        <v>1</v>
-      </c>
-      <c r="AH6">
         <v>1</v>
       </c>
     </row>
@@ -8588,7 +8585,7 @@
         <v>0</v>
       </c>
       <c r="W75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y75" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
Correction of documentation for some entries of reason_for_exclusion in study_set files.
</commit_message>
<xml_diff>
--- a/data/study_search/database_search/processed/post_AS/packages_for_full_text_download/study_set_14.xlsx
+++ b/data/study_search/database_search/processed/post_AS/packages_for_full_text_download/study_set_14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franzprante/GitHub/MORPEP/META_CMP/data/data/study_search/database_search/processed/post_AS/packages_for_full_text_download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E1B1143-75BE-894B-8D86-280249C9ECD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896137D0-7C16-0543-9DE3-7AA799EE1CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="20520" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="898">
   <si>
     <t>record_id</t>
   </si>
@@ -2754,6 +2754,9 @@
   </si>
   <si>
     <t>full_random_check</t>
+  </si>
+  <si>
+    <t>effect_size_unclear</t>
   </si>
 </sst>
 </file>
@@ -3094,8 +3097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V39" zoomScale="125" zoomScaleNormal="83" workbookViewId="0">
-      <selection activeCell="AC53" sqref="AC53"/>
+    <sheetView tabSelected="1" topLeftCell="T55" zoomScale="125" zoomScaleNormal="83" workbookViewId="0">
+      <selection activeCell="X75" sqref="X75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.83203125" defaultRowHeight="15"/>
@@ -7966,7 +7969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:32">
+    <row r="65" spans="1:31">
       <c r="A65">
         <v>10068</v>
       </c>
@@ -8043,7 +8046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:32">
+    <row r="66" spans="1:31">
       <c r="A66">
         <v>6965</v>
       </c>
@@ -8105,7 +8108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:32">
+    <row r="67" spans="1:31">
       <c r="A67">
         <v>5340</v>
       </c>
@@ -8182,7 +8185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:32">
+    <row r="68" spans="1:31">
       <c r="A68">
         <v>848</v>
       </c>
@@ -8250,7 +8253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:32">
+    <row r="69" spans="1:31">
       <c r="A69">
         <v>4066</v>
       </c>
@@ -8324,7 +8327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:32">
+    <row r="70" spans="1:31">
       <c r="A70">
         <v>7038</v>
       </c>
@@ -8392,7 +8395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:32">
+    <row r="71" spans="1:31">
       <c r="A71">
         <v>6428</v>
       </c>
@@ -8466,7 +8469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:32">
+    <row r="72" spans="1:31">
       <c r="A72">
         <v>3884</v>
       </c>
@@ -8540,7 +8543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:32">
+    <row r="73" spans="1:31">
       <c r="A73">
         <v>10367</v>
       </c>
@@ -8617,7 +8620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:32">
+    <row r="74" spans="1:31">
       <c r="A74">
         <v>7055</v>
       </c>
@@ -8694,7 +8697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:32">
+    <row r="75" spans="1:31">
       <c r="A75">
         <v>10666</v>
       </c>
@@ -8746,17 +8749,26 @@
       <c r="W75">
         <v>0</v>
       </c>
+      <c r="X75" t="s">
+        <v>897</v>
+      </c>
       <c r="Y75" t="s">
         <v>45</v>
       </c>
+      <c r="Z75" t="s">
+        <v>489</v>
+      </c>
+      <c r="AB75">
+        <v>1</v>
+      </c>
+      <c r="AC75" t="s">
+        <v>892</v>
+      </c>
       <c r="AE75">
         <v>1</v>
       </c>
-      <c r="AF75" t="s">
-        <v>893</v>
-      </c>
     </row>
-    <row r="76" spans="1:32">
+    <row r="76" spans="1:31">
       <c r="A76">
         <v>7823</v>
       </c>
@@ -8833,7 +8845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:32">
+    <row r="77" spans="1:31">
       <c r="A77">
         <v>10147</v>
       </c>
@@ -8910,7 +8922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:32" ht="16">
+    <row r="78" spans="1:31" ht="16">
       <c r="A78">
         <v>8240</v>
       </c>
@@ -8978,7 +8990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:32">
+    <row r="79" spans="1:31">
       <c r="A79">
         <v>7362</v>
       </c>
@@ -9052,7 +9064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:32">
+    <row r="80" spans="1:31">
       <c r="A80">
         <v>10078</v>
       </c>

</xml_diff>